<commit_message>
Report finalised, hyperlinking pending
</commit_message>
<xml_diff>
--- a/documentation/Project Report/report.xlsx
+++ b/documentation/Project Report/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UCD\coursework\S2\Software Engineering\projects and assignment\UCD_CSconv_DublinBike\documentation\Project Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F487DA46-A5B8-4201-BD24-306AE304C754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA80A1F6-E653-40D9-8A88-0A891AF15035}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>PARAMETER</t>
   </si>
@@ -76,6 +76,54 @@
   </si>
   <si>
     <t>wind_deg</t>
+  </si>
+  <si>
+    <t>Joshi Omkar</t>
+  </si>
+  <si>
+    <t>Kane Rasik</t>
+  </si>
+  <si>
+    <t>Keshwar Ratnaprabha</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Contribution</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Reasons for shortcomings</t>
+  </si>
+  <si>
+    <t>Designed Front End
+Designed server infrastructure</t>
+  </si>
+  <si>
+    <t>Designed Database architecture 
+Designed webAPI Scraper
+Designed ML models for prediction</t>
+  </si>
+  <si>
+    <t>Contributed to Database design
+Contributed to ML model design philosophy
+Designed UI Wireframes
+Contributed to UI design</t>
+  </si>
+  <si>
+    <t>Returned home and was quarantined for 2 week
+Faced challenges with ML - UI integration</t>
+  </si>
+  <si>
+    <t>Returned home and was hospitalised for 2 week
+Faced queries regarding weather ML model design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faced challenges with scraper optimization
+Faced problems regarding ML model optimization </t>
   </si>
 </sst>
 </file>
@@ -145,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -161,6 +209,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,18 +499,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E13"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -662,6 +719,62 @@
         <v>0.901932654</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>